<commit_message>
added samples to fastq file
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_01.19.21.xlsx
+++ b/fastqFiles/fastq_01.19.21.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A589EF-D5D5-A348-9F50-61CCFE428D2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B296446B-0049-E042-ABB5-02069DE58B3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{A35C8EC1-BE76-D94E-970E-A92E428D437D}"/>
+    <workbookView xWindow="4520" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{A35C8EC1-BE76-D94E-970E-A92E428D437D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="107">
   <si>
     <t>libraryDate</t>
   </si>
@@ -139,6 +139,213 @@
   </si>
   <si>
     <t>Brent_24_GTAC_24_SIC_Index2_07_GGAGTCC_GAGTTGGT_S57_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>01.09.21</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Brent_DA_19_GTAC_1_SIC_Index2_10_TGAGGTT_GCTTCTGT_S26_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_20_GTAC_2_SIC_Index2_10_GCTTAGA_GCTTCTGT_S27_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_21_GTAC_3_SIC_Index2_10_ATGACAG_GCTTCTGT_S28_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_22_GTAC_4_SIC_Index2_10_CACCTCC_GCTTCTGT_S29_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_23_GTAC_5_SIC_Index2_10_ATCGAGC_GCTTCTGT_S30_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_24_GTAC_6_SIC_Index2_10_TACTCTA_GCTTCTGT_S31_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_25_GTAC_7_SIC_Index2_10_AGACTGA_GCTTCTGT_S32_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_26_GTAC_8_SIC_Index2_10_CTTGGAA_GCTTCTGT_S33_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_27_GTAC_9_SIC_Index2_10_CCGATTA_GCTTCTGT_S34_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_28_GTAC_10_SIC_Index2_10_GGCAGCG_GCTTCTGT_S35_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_29_GTAC_11_SIC_Index2_10_CCATCAT_GCTTCTGT_S36_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_30_GTAC_12_SIC_Index2_10_TAACAAG_GCTTCTGT_S37_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_31_GTAC_13_SIC_Index2_10_GAGGCGT_GCTTCTGT_S38_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_32_GTAC_14_SIC_Index2_10_TTTAACT_GCTTCTGT_S39_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_33_GTAC_15_SIC_Index2_10_GGTCCTC_GCTTCTGT_S40_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_34_GTAC_16_SIC_Index2_10_CGGTGGC_GCTTCTGT_S41_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_35_GTAC_17_SIC_Index2_10_ACTGTCG_GCTTCTGT_S42_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_36_GTAC_18_SIC_Index2_10_GTATTTG_GCTTCTGT_S43_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_37_GTAC_19_SIC_Index2_10_GAGTACG_GCTTCTGT_S44_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_38_GTAC_20_SIC_Index2_10_ACAGATA_GCTTCTGT_S45_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_39_GTAC_21_SIC_Index2_10_CTCAATG_GCTTCTGT_S46_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_40_GTAC_22_SIC_Index2_10_AAATGCA_GCTTCTGT_S47_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_41_GTAC_23_SIC_Index2_10_ACGCGGG_GCTTCTGT_S48_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_42_GTAC_24_SIC_Index2_10_GGAGTCC_GCTTCTGT_S49_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_43_GTAC_25_SIC_Index2_10_CGTCGCT_GCTTCTGT_S50_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_44_GTAC_26_SIC_Index2_10_TCAACTG_GCTTCTGT_S51_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_45_GTAC_27_SIC_Index2_10_TGTTTGT_GCTTCTGT_S52_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_46_GTAC_28_SIC_Index2_10_TACATGG_GCTTCTGT_S53_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_47_GTAC_29_SIC_Index2_10_GTTCTCA_GCTTCTGT_S54_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_48_GTAC_30_SIC_Index2_10_CTGGTGG_GCTTCTGT_S55_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_49_GTAC_31_SIC_Index2_10_TGCCCAT_GCTTCTGT_S56_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_50_GTAC_32_SIC_Index2_10_AAACCTT_GCTTCTGT_S57_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_51_GTAC_33_SIC_Index2_10_ACCATAC_GCTTCTGT_S58_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_52_GTAC_41_SIC_Index2_10_TTGCCCC_GCTTCTGT_S59_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_53_GTAC_42_SIC_Index2_10_ACTCCAA_GCTTCTGT_S60_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_54_GTAC_43_SIC_Index2_10_TGTGCCA_GCTTCTGT_S61_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_55_GTAC_37_SIC_Index2_10_TTTTGTC_GCTTCTGT_S62_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_56_GTAC_38_SIC_Index2_10_ACCCACT_GCTTCTGT_S63_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_57_GTAC_39_SIC_Index2_10_CCGGACC_GCTTCTGT_S64_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_DA_58_GTAC_40_SIC_Index2_10_GTACGGC_GCTTCTGT_S65_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_1_GTAC_1_SIC_Index2_06_TGAGGTT_GACCTTGT_S66_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_2_GTAC_2_SIC_Index2_06_GCTTAGA_GACCTTGT_S67_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_3_GTAC_3_SIC_Index2_06_ATGACAG_GACCTTGT_S68_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_4_GTAC_4_SIC_Index2_06_CACCTCC_GACCTTGT_S69_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_5_GTAC_5_SIC_Index2_06_ATCGAGC_GACCTTGT_S70_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_6_GTAC_6_SIC_Index2_06_TACTCTA_GACCTTGT_S71_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_7_GTAC_7_SIC_Index2_06_AGACTGA_GACCTTGT_S72_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_8_GTAC_8_SIC_Index2_06_CTTGGAA_GACCTTGT_S73_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_9_GTAC_9_SIC_Index2_06_CCGATTA_GACCTTGT_S74_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_10_GTAC_10_SIC_Index2_06_GGCAGCG_GACCTTGT_S75_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_11_GTAC_11_SIC_Index2_06_CCATCAT_GACCTTGT_S76_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_12_GTAC_12_SIC_Index2_06_TAACAAG_GACCTTGT_S77_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_13_GTAC_13_SIC_Index2_06_GAGGCGT_GACCTTGT_S78_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_14_GTAC_14_SIC_Index2_06_TTTAACT_GACCTTGT_S79_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_15_GTAC_15_SIC_Index2_06_GGTCCTC_GACCTTGT_S80_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_16_GTAC_16_SIC_Index2_06_CGGTGGC_GACCTTGT_S81_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_17_GTAC_17_SIC_Index2_06_ACTGTCG_GACCTTGT_S82_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_18_GTAC_18_SIC_Index2_06_GTATTTG_GACCTTGT_S83_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_19_GTAC_19_SIC_Index2_06_GAGTACG_GACCTTGT_S84_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_20_GTAC_20_SIC_Index2_06_ACAGATA_GACCTTGT_S85_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_21_GTAC_21_SIC_Index2_06_CTCAATG_GACCTTGT_S86_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_22_GTAC_22_SIC_Index2_06_AAATGCA_GACCTTGT_S87_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_23_GTAC_23_SIC_Index2_06_ACGCGGG_GACCTTGT_S88_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_24_GTAC_24_SIC_Index2_06_GGAGTCC_GACCTTGT_S89_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_25_GTAC_25_SIC_Index2_06_CGTCGCT_GACCTTGT_S90_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2e_26_GTAC_26_SIC_Index2_06_TCAACTG_GACCTTGT_S91_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>12.22.20</t>
   </si>
 </sst>
 </file>
@@ -490,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48740E37-0308-7B4C-A9FF-1EBEA525511A}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="Q75" sqref="Q75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1298,6 +1505,2118 @@
         <v>37</v>
       </c>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>4783</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26">
+        <v>45788</v>
+      </c>
+      <c r="J26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>4783</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>46842</v>
+      </c>
+      <c r="J27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>4783</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28">
+        <v>76258</v>
+      </c>
+      <c r="J28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>4783</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29">
+        <v>5</v>
+      </c>
+      <c r="I29">
+        <v>41704</v>
+      </c>
+      <c r="J29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>4783</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+      <c r="I30">
+        <v>26929</v>
+      </c>
+      <c r="J30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>4783</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31">
+        <v>36327</v>
+      </c>
+      <c r="J31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>4783</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+      <c r="I32">
+        <v>47445</v>
+      </c>
+      <c r="J32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <v>4783</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+      <c r="I33">
+        <v>33532</v>
+      </c>
+      <c r="J33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>9</v>
+      </c>
+      <c r="D34">
+        <v>4783</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34">
+        <v>5</v>
+      </c>
+      <c r="I34">
+        <v>56679</v>
+      </c>
+      <c r="J34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>4783</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35">
+        <v>5</v>
+      </c>
+      <c r="I35">
+        <v>21914</v>
+      </c>
+      <c r="J35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>11</v>
+      </c>
+      <c r="D36">
+        <v>4783</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36">
+        <v>5</v>
+      </c>
+      <c r="I36">
+        <v>18082</v>
+      </c>
+      <c r="J36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>4783</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37">
+        <v>5</v>
+      </c>
+      <c r="I37">
+        <v>10252</v>
+      </c>
+      <c r="J37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>4783</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+      <c r="I38">
+        <v>11118</v>
+      </c>
+      <c r="J38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>14</v>
+      </c>
+      <c r="D39">
+        <v>4783</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39">
+        <v>5</v>
+      </c>
+      <c r="I39">
+        <v>16320</v>
+      </c>
+      <c r="J39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>15</v>
+      </c>
+      <c r="D40">
+        <v>4783</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40">
+        <v>5</v>
+      </c>
+      <c r="I40">
+        <v>10792</v>
+      </c>
+      <c r="J40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>4783</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41">
+        <v>5</v>
+      </c>
+      <c r="I41">
+        <v>12080</v>
+      </c>
+      <c r="J41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>17</v>
+      </c>
+      <c r="D42">
+        <v>4783</v>
+      </c>
+      <c r="E42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42">
+        <v>5</v>
+      </c>
+      <c r="I42">
+        <v>13433</v>
+      </c>
+      <c r="J42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <v>18</v>
+      </c>
+      <c r="D43">
+        <v>4783</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43">
+        <v>5</v>
+      </c>
+      <c r="I43">
+        <v>31286</v>
+      </c>
+      <c r="J43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>19</v>
+      </c>
+      <c r="D44">
+        <v>4783</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
+      <c r="I44">
+        <v>15329</v>
+      </c>
+      <c r="J44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>20</v>
+      </c>
+      <c r="D45">
+        <v>4783</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+      <c r="I45">
+        <v>32387</v>
+      </c>
+      <c r="J45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46">
+        <v>21</v>
+      </c>
+      <c r="D46">
+        <v>4783</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46">
+        <v>3.0303030303030303</v>
+      </c>
+      <c r="I46">
+        <v>1090</v>
+      </c>
+      <c r="J46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47">
+        <v>22</v>
+      </c>
+      <c r="D47">
+        <v>4783</v>
+      </c>
+      <c r="E47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47">
+        <v>3.5335689045936394</v>
+      </c>
+      <c r="I47">
+        <v>9125</v>
+      </c>
+      <c r="J47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>23</v>
+      </c>
+      <c r="D48">
+        <v>4783</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" t="s">
+        <v>39</v>
+      </c>
+      <c r="I48">
+        <v>20146</v>
+      </c>
+      <c r="J48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49">
+        <v>24</v>
+      </c>
+      <c r="D49">
+        <v>4783</v>
+      </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49">
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="I49">
+        <v>13595</v>
+      </c>
+      <c r="J49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50">
+        <v>25</v>
+      </c>
+      <c r="D50">
+        <v>4783</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" t="s">
+        <v>39</v>
+      </c>
+      <c r="I50">
+        <v>9712</v>
+      </c>
+      <c r="J50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51">
+        <v>26</v>
+      </c>
+      <c r="D51">
+        <v>4783</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <v>12216</v>
+      </c>
+      <c r="J51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52">
+        <v>27</v>
+      </c>
+      <c r="D52">
+        <v>4783</v>
+      </c>
+      <c r="E52" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52">
+        <v>5</v>
+      </c>
+      <c r="I52">
+        <v>11488</v>
+      </c>
+      <c r="J52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <v>28</v>
+      </c>
+      <c r="D53">
+        <v>4783</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53">
+        <v>1.044932079414838</v>
+      </c>
+      <c r="I53">
+        <v>15406</v>
+      </c>
+      <c r="J53" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54">
+        <v>29</v>
+      </c>
+      <c r="D54">
+        <v>4783</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54">
+        <v>1.5748031496062993</v>
+      </c>
+      <c r="I54">
+        <v>13548</v>
+      </c>
+      <c r="J54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55">
+        <v>30</v>
+      </c>
+      <c r="D55">
+        <v>4783</v>
+      </c>
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" t="s">
+        <v>39</v>
+      </c>
+      <c r="I55">
+        <v>18759</v>
+      </c>
+      <c r="J55" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56">
+        <v>31</v>
+      </c>
+      <c r="D56">
+        <v>4783</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" t="s">
+        <v>39</v>
+      </c>
+      <c r="I56">
+        <v>18555</v>
+      </c>
+      <c r="J56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <v>32</v>
+      </c>
+      <c r="D57">
+        <v>4783</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" t="s">
+        <v>39</v>
+      </c>
+      <c r="I57">
+        <v>20055</v>
+      </c>
+      <c r="J57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58">
+        <v>33</v>
+      </c>
+      <c r="D58">
+        <v>4783</v>
+      </c>
+      <c r="E58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" t="s">
+        <v>39</v>
+      </c>
+      <c r="I58">
+        <v>31602</v>
+      </c>
+      <c r="J58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59">
+        <v>34</v>
+      </c>
+      <c r="D59">
+        <v>4783</v>
+      </c>
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59">
+        <v>5</v>
+      </c>
+      <c r="I59">
+        <v>20083</v>
+      </c>
+      <c r="J59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60">
+        <v>35</v>
+      </c>
+      <c r="D60">
+        <v>4783</v>
+      </c>
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" t="s">
+        <v>39</v>
+      </c>
+      <c r="I60">
+        <v>12504</v>
+      </c>
+      <c r="J60" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61">
+        <v>36</v>
+      </c>
+      <c r="D61">
+        <v>4783</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" t="s">
+        <v>13</v>
+      </c>
+      <c r="H61" t="s">
+        <v>39</v>
+      </c>
+      <c r="I61">
+        <v>10464</v>
+      </c>
+      <c r="J61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62">
+        <v>37</v>
+      </c>
+      <c r="D62">
+        <v>4783</v>
+      </c>
+      <c r="E62" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H62">
+        <v>5</v>
+      </c>
+      <c r="I62">
+        <v>7176</v>
+      </c>
+      <c r="J62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63">
+        <v>38</v>
+      </c>
+      <c r="D63">
+        <v>4783</v>
+      </c>
+      <c r="E63" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" t="s">
+        <v>13</v>
+      </c>
+      <c r="H63" t="s">
+        <v>39</v>
+      </c>
+      <c r="I63">
+        <v>11396</v>
+      </c>
+      <c r="J63" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64">
+        <v>39</v>
+      </c>
+      <c r="D64">
+        <v>4783</v>
+      </c>
+      <c r="E64" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" t="s">
+        <v>13</v>
+      </c>
+      <c r="H64" t="s">
+        <v>39</v>
+      </c>
+      <c r="I64">
+        <v>12159</v>
+      </c>
+      <c r="J64" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65">
+        <v>40</v>
+      </c>
+      <c r="D65">
+        <v>4783</v>
+      </c>
+      <c r="E65" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" t="s">
+        <v>39</v>
+      </c>
+      <c r="I65">
+        <v>9357</v>
+      </c>
+      <c r="J65" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>4783</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" t="s">
+        <v>13</v>
+      </c>
+      <c r="H66">
+        <v>5</v>
+      </c>
+      <c r="I66">
+        <v>27998</v>
+      </c>
+      <c r="J66" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>4783</v>
+      </c>
+      <c r="E67" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" t="s">
+        <v>13</v>
+      </c>
+      <c r="H67">
+        <v>1.5503875968992247</v>
+      </c>
+      <c r="I67">
+        <v>1031</v>
+      </c>
+      <c r="J67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>106</v>
+      </c>
+      <c r="B68" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68">
+        <v>4783</v>
+      </c>
+      <c r="E68" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" t="s">
+        <v>13</v>
+      </c>
+      <c r="H68">
+        <v>5</v>
+      </c>
+      <c r="I68">
+        <v>17383</v>
+      </c>
+      <c r="J68" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>106</v>
+      </c>
+      <c r="B69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>4783</v>
+      </c>
+      <c r="E69" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" t="s">
+        <v>13</v>
+      </c>
+      <c r="H69">
+        <v>5</v>
+      </c>
+      <c r="I69">
+        <v>7890</v>
+      </c>
+      <c r="J69" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
+      </c>
+      <c r="D70">
+        <v>4783</v>
+      </c>
+      <c r="E70" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" t="s">
+        <v>13</v>
+      </c>
+      <c r="H70">
+        <v>5</v>
+      </c>
+      <c r="I70">
+        <v>5459</v>
+      </c>
+      <c r="J70" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71">
+        <v>6</v>
+      </c>
+      <c r="D71">
+        <v>4783</v>
+      </c>
+      <c r="E71" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G71" t="s">
+        <v>13</v>
+      </c>
+      <c r="H71">
+        <v>5</v>
+      </c>
+      <c r="I71">
+        <v>6255</v>
+      </c>
+      <c r="J71" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72">
+        <v>7</v>
+      </c>
+      <c r="D72">
+        <v>4783</v>
+      </c>
+      <c r="E72" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" t="s">
+        <v>13</v>
+      </c>
+      <c r="H72">
+        <v>5</v>
+      </c>
+      <c r="I72">
+        <v>12946</v>
+      </c>
+      <c r="J72" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>106</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73">
+        <v>8</v>
+      </c>
+      <c r="D73">
+        <v>4783</v>
+      </c>
+      <c r="E73" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" t="s">
+        <v>13</v>
+      </c>
+      <c r="H73">
+        <v>5</v>
+      </c>
+      <c r="I73">
+        <v>13616</v>
+      </c>
+      <c r="J73" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>106</v>
+      </c>
+      <c r="B74" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74">
+        <v>9</v>
+      </c>
+      <c r="D74">
+        <v>4783</v>
+      </c>
+      <c r="E74" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" t="s">
+        <v>12</v>
+      </c>
+      <c r="G74" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74">
+        <v>0.8771929824561403</v>
+      </c>
+      <c r="I74">
+        <v>13325</v>
+      </c>
+      <c r="J74" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>106</v>
+      </c>
+      <c r="B75" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75">
+        <v>10</v>
+      </c>
+      <c r="D75">
+        <v>4783</v>
+      </c>
+      <c r="E75" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75">
+        <v>1.7985611510791368</v>
+      </c>
+      <c r="I75">
+        <v>10436</v>
+      </c>
+      <c r="J75" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>106</v>
+      </c>
+      <c r="B76" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76">
+        <v>11</v>
+      </c>
+      <c r="D76">
+        <v>4783</v>
+      </c>
+      <c r="E76" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" t="s">
+        <v>13</v>
+      </c>
+      <c r="H76">
+        <v>1.0245901639344261</v>
+      </c>
+      <c r="I76">
+        <v>15813</v>
+      </c>
+      <c r="J76" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>106</v>
+      </c>
+      <c r="B77" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77">
+        <v>12</v>
+      </c>
+      <c r="D77">
+        <v>4783</v>
+      </c>
+      <c r="E77" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" t="s">
+        <v>13</v>
+      </c>
+      <c r="H77">
+        <v>3.3444816053511701</v>
+      </c>
+      <c r="I77">
+        <v>13548</v>
+      </c>
+      <c r="J77" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>106</v>
+      </c>
+      <c r="B78" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78">
+        <v>13</v>
+      </c>
+      <c r="D78">
+        <v>4783</v>
+      </c>
+      <c r="E78" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" t="s">
+        <v>13</v>
+      </c>
+      <c r="H78">
+        <v>3.5211267605633805</v>
+      </c>
+      <c r="I78">
+        <v>15219</v>
+      </c>
+      <c r="J78" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>106</v>
+      </c>
+      <c r="B79" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79">
+        <v>14</v>
+      </c>
+      <c r="D79">
+        <v>4783</v>
+      </c>
+      <c r="E79" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" t="s">
+        <v>13</v>
+      </c>
+      <c r="H79">
+        <v>5</v>
+      </c>
+      <c r="I79">
+        <v>57942</v>
+      </c>
+      <c r="J79" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80">
+        <v>15</v>
+      </c>
+      <c r="D80">
+        <v>4783</v>
+      </c>
+      <c r="E80" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" t="s">
+        <v>13</v>
+      </c>
+      <c r="H80">
+        <v>0.70422535211267612</v>
+      </c>
+      <c r="I80">
+        <v>13619</v>
+      </c>
+      <c r="J80" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>106</v>
+      </c>
+      <c r="B81" t="s">
+        <v>11</v>
+      </c>
+      <c r="C81">
+        <v>16</v>
+      </c>
+      <c r="D81">
+        <v>4783</v>
+      </c>
+      <c r="E81" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" t="s">
+        <v>13</v>
+      </c>
+      <c r="H81">
+        <v>5</v>
+      </c>
+      <c r="I81">
+        <v>108887</v>
+      </c>
+      <c r="J81" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82">
+        <v>17</v>
+      </c>
+      <c r="D82">
+        <v>4783</v>
+      </c>
+      <c r="E82" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" t="s">
+        <v>13</v>
+      </c>
+      <c r="H82">
+        <v>0.77519379844961234</v>
+      </c>
+      <c r="I82">
+        <v>12155</v>
+      </c>
+      <c r="J82" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>106</v>
+      </c>
+      <c r="B83" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83">
+        <v>18</v>
+      </c>
+      <c r="D83">
+        <v>4783</v>
+      </c>
+      <c r="E83" t="s">
+        <v>12</v>
+      </c>
+      <c r="F83" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" t="s">
+        <v>13</v>
+      </c>
+      <c r="H83">
+        <v>1.6181229773462784</v>
+      </c>
+      <c r="I83">
+        <v>13181</v>
+      </c>
+      <c r="J83" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>106</v>
+      </c>
+      <c r="B84" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84">
+        <v>19</v>
+      </c>
+      <c r="D84">
+        <v>4783</v>
+      </c>
+      <c r="E84" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" t="s">
+        <v>13</v>
+      </c>
+      <c r="H84">
+        <v>1.9047619047619047</v>
+      </c>
+      <c r="I84">
+        <v>11621</v>
+      </c>
+      <c r="J84" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>106</v>
+      </c>
+      <c r="B85" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85">
+        <v>20</v>
+      </c>
+      <c r="D85">
+        <v>4783</v>
+      </c>
+      <c r="E85" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85" t="s">
+        <v>13</v>
+      </c>
+      <c r="H85">
+        <v>1.9120458891013383</v>
+      </c>
+      <c r="I85">
+        <v>11488</v>
+      </c>
+      <c r="J85" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>106</v>
+      </c>
+      <c r="B86" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86">
+        <v>21</v>
+      </c>
+      <c r="D86">
+        <v>4783</v>
+      </c>
+      <c r="E86" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" t="s">
+        <v>13</v>
+      </c>
+      <c r="H86">
+        <v>5</v>
+      </c>
+      <c r="I86">
+        <v>18713</v>
+      </c>
+      <c r="J86" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>106</v>
+      </c>
+      <c r="B87" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87">
+        <v>22</v>
+      </c>
+      <c r="D87">
+        <v>4783</v>
+      </c>
+      <c r="E87" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" t="s">
+        <v>12</v>
+      </c>
+      <c r="G87" t="s">
+        <v>13</v>
+      </c>
+      <c r="H87">
+        <v>5</v>
+      </c>
+      <c r="I87">
+        <v>6012</v>
+      </c>
+      <c r="J87" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>106</v>
+      </c>
+      <c r="B88" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88">
+        <v>23</v>
+      </c>
+      <c r="D88">
+        <v>4783</v>
+      </c>
+      <c r="E88" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G88" t="s">
+        <v>13</v>
+      </c>
+      <c r="H88">
+        <v>5</v>
+      </c>
+      <c r="I88">
+        <v>18293</v>
+      </c>
+      <c r="J88" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>106</v>
+      </c>
+      <c r="B89" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89">
+        <v>24</v>
+      </c>
+      <c r="D89">
+        <v>4783</v>
+      </c>
+      <c r="E89" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89">
+        <v>5</v>
+      </c>
+      <c r="I89">
+        <v>16751</v>
+      </c>
+      <c r="J89" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>106</v>
+      </c>
+      <c r="B90" t="s">
+        <v>11</v>
+      </c>
+      <c r="C90">
+        <v>25</v>
+      </c>
+      <c r="D90">
+        <v>4783</v>
+      </c>
+      <c r="E90" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90">
+        <v>5</v>
+      </c>
+      <c r="I90">
+        <v>64588</v>
+      </c>
+      <c r="J90" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>106</v>
+      </c>
+      <c r="B91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C91">
+        <v>26</v>
+      </c>
+      <c r="D91">
+        <v>4783</v>
+      </c>
+      <c r="E91" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" t="s">
+        <v>12</v>
+      </c>
+      <c r="G91" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91">
+        <v>5</v>
+      </c>
+      <c r="I91">
+        <v>69854</v>
+      </c>
+      <c r="J91" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>